<commit_message>
Previous commit did not grab changes
</commit_message>
<xml_diff>
--- a/bcd/CREST/Appliance/Determining_Appliance_Inputs.xlsx
+++ b/bcd/CREST/Appliance/Determining_Appliance_Inputs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
   <si>
     <t>Appliance</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>DOE Energy</t>
+  </si>
+  <si>
+    <t>Average of &gt;42" and &lt;42"</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1097,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,6 +1359,9 @@
       <c r="F12" s="21">
         <v>401</v>
       </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
@@ -1367,9 +1373,18 @@
       <c r="C13" s="27">
         <v>4</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="20">
+        <v>168</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>401</v>
+      </c>
+      <c r="G13" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
@@ -1401,9 +1416,15 @@
       <c r="C15" s="27">
         <v>4</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="21"/>
+      <c r="D15" s="20">
+        <v>168</v>
+      </c>
+      <c r="E15" s="19">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21">
+        <v>401</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">

</xml_diff>